<commit_message>
updated code and files
</commit_message>
<xml_diff>
--- a/tests/data/test_files/stm_most_popular_plans.xlsx
+++ b/tests/data/test_files/stm_most_popular_plans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optum\hm-automation\tests\data\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5E9B66-5ABC-4DFC-99A7-56F3019AA79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D4A745-2291-4C51-B7BC-0D8B94F9207C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E59AB3A4-B2E1-4FD6-A202-BD117C9D2742}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E59AB3A4-B2E1-4FD6-A202-BD117C9D2742}"/>
   </bookViews>
   <sheets>
     <sheet name="STM Popular plans" sheetId="2" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Test Results'!$H$1:$H$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1577,7 +1578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B126BD7-6732-4E02-9E85-5975E0BE5B14}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -1999,9 +2000,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C248C016-80C0-4B89-9687-8882F2E37C0B}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -2047,7 +2049,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17">
         <v>85001</v>
       </c>
@@ -2071,7 +2073,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <v>85321</v>
       </c>
@@ -2100,7 +2102,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>33004</v>
       </c>
@@ -2125,7 +2127,7 @@
       </c>
       <c r="I4" s="26"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>33002</v>
       </c>
@@ -2149,7 +2151,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
         <v>33401</v>
       </c>
@@ -2173,7 +2175,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>33710</v>
       </c>
@@ -2197,7 +2199,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>30004</v>
       </c>
@@ -2224,7 +2226,7 @@
       </c>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>30003</v>
       </c>
@@ -2248,7 +2250,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>60018</v>
       </c>
@@ -2272,7 +2274,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
         <v>60126</v>
       </c>
@@ -2327,7 +2329,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>46040</v>
       </c>
@@ -2354,7 +2356,7 @@
       </c>
       <c r="I13" s="26"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>46106</v>
       </c>
@@ -2381,7 +2383,7 @@
       </c>
       <c r="I14" s="26"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <v>46113</v>
       </c>
@@ -2410,7 +2412,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <v>46613</v>
       </c>
@@ -2463,7 +2465,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>48070</v>
       </c>
@@ -2487,7 +2489,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>55311</v>
       </c>
@@ -2512,7 +2514,7 @@
       </c>
       <c r="I19" s="22"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>38611</v>
       </c>
@@ -2539,7 +2541,7 @@
       </c>
       <c r="I20" s="26"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>64024</v>
       </c>
@@ -2566,7 +2568,7 @@
       </c>
       <c r="I21" s="26"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>64002</v>
       </c>
@@ -2590,7 +2592,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>63301</v>
       </c>
@@ -2614,7 +2616,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>63005</v>
       </c>
@@ -2641,7 +2643,7 @@
       </c>
       <c r="I24" s="26"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>65614</v>
       </c>
@@ -2668,7 +2670,7 @@
       </c>
       <c r="I25" s="26"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>68007</v>
       </c>
@@ -2697,7 +2699,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>68317</v>
       </c>
@@ -2782,7 +2784,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
         <v>44022</v>
       </c>
@@ -2811,7 +2813,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19">
         <v>43003</v>
       </c>
@@ -2840,7 +2842,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="19">
         <v>43046</v>
       </c>
@@ -2867,7 +2869,7 @@
       </c>
       <c r="I32" s="26"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="19">
         <v>43081</v>
       </c>
@@ -2893,7 +2895,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="19">
         <v>44001</v>
       </c>
@@ -2917,7 +2919,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19">
         <v>44212</v>
       </c>
@@ -2941,7 +2943,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="19">
         <v>44601</v>
       </c>
@@ -2968,7 +2970,7 @@
       </c>
       <c r="I36" s="26"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19">
         <v>44301</v>
       </c>
@@ -2992,7 +2994,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="19">
         <v>44214</v>
       </c>
@@ -3018,7 +3020,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20">
         <v>73019</v>
       </c>
@@ -3041,7 +3043,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="20">
         <v>73003</v>
       </c>
@@ -3068,7 +3070,7 @@
       </c>
       <c r="I40" s="26"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20">
         <v>74008</v>
       </c>
@@ -3095,7 +3097,7 @@
       </c>
       <c r="I41" s="26"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20">
         <v>15006</v>
       </c>
@@ -3119,7 +3121,7 @@
       </c>
       <c r="I42" s="22"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20">
         <v>19301</v>
       </c>
@@ -3143,7 +3145,7 @@
       </c>
       <c r="I43" s="22"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20">
         <v>18011</v>
       </c>
@@ -3170,7 +3172,7 @@
       </c>
       <c r="I44" s="26"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20">
         <v>18001</v>
       </c>
@@ -3193,7 +3195,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20">
         <v>15062</v>
       </c>
@@ -3217,7 +3219,7 @@
       </c>
       <c r="I46" s="22"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="20">
         <v>37011</v>
       </c>
@@ -3240,7 +3242,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20">
         <v>37721</v>
       </c>
@@ -3267,7 +3269,7 @@
       </c>
       <c r="I48" s="26"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20">
         <v>77001</v>
       </c>
@@ -3291,7 +3293,7 @@
       </c>
       <c r="I49" s="26"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20">
         <v>76009</v>
       </c>
@@ -3314,7 +3316,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20">
         <v>76001</v>
       </c>
@@ -3364,7 +3366,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="H1:H52" xr:uid="{C248C016-80C0-4B89-9687-8882F2E37C0B}"/>
+  <autoFilter ref="H1:H52" xr:uid="{C248C016-80C0-4B89-9687-8882F2E37C0B}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="FAILED"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>